<commit_message>
add chapter 6 of pythonprograming
</commit_message>
<xml_diff>
--- a/Python2.7/Python summary-filter.xlsx
+++ b/Python2.7/Python summary-filter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="7965" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="7965" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -952,7 +952,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="2294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2740" uniqueCount="2297">
   <si>
     <t>Python教程</t>
   </si>
@@ -13320,6 +13320,17 @@
 &gt;&gt;&gt; del aList[1]
 &gt;&gt;&gt; aList
 [[1, [2, [3, 7]]]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> max(iter, key = None) or
+max(arg0, arg1, ..., key = None) 返回iter或（arg0, arg1...）中的最大值，如果指定了key,这个key必须是一个可以传给sort（）方法的，用于比较多回调函数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> min(iter, key = None) or
+min(arg0, arg1, ..., key = None) 返回iter或（arg0, arg1...）中的最小值，如果指定了key,这个key必须是一个可以传给sort（）方法的，用于比较多回调函数 </t>
+  </si>
+  <si>
+    <t>sum(seq, init = 0) 返回seq和可选参数init的总和</t>
   </si>
 </sst>
 </file>
@@ -14502,7 +14513,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -15061,7 +15072,16 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -15070,49 +15090,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="53" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="54" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15136,6 +15126,9 @@
     <xf numFmtId="0" fontId="29" fillId="4" borderId="59" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -15148,11 +15141,38 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="52" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="51" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -15162,12 +15182,6 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -16729,7 +16743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
@@ -17125,18 +17139,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="187" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
-      <c r="G1" s="190"/>
-      <c r="H1" s="190"/>
-      <c r="I1" s="190"/>
-      <c r="J1" s="190"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
     </row>
     <row r="2" spans="1:10" ht="16.5">
       <c r="A2" s="7" t="s">
@@ -17158,33 +17172,33 @@
       <c r="A3" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="187" t="s">
+      <c r="B3" s="190" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="187"/>
-      <c r="D3" s="187"/>
-      <c r="E3" s="187"/>
-      <c r="F3" s="187"/>
-      <c r="G3" s="187"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="187"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
     </row>
     <row r="4" spans="1:10" ht="16.5">
       <c r="A4" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="187" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="190"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="190"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
     </row>
     <row r="5" spans="1:10" ht="16.5">
       <c r="A5" s="7" t="s">
@@ -17206,17 +17220,17 @@
       <c r="A6" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="187" t="s">
+      <c r="B6" s="190" t="s">
         <v>203</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
+      <c r="C6" s="190"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="190"/>
+      <c r="F6" s="190"/>
+      <c r="G6" s="190"/>
+      <c r="H6" s="190"/>
+      <c r="I6" s="190"/>
+      <c r="J6" s="190"/>
     </row>
     <row r="7" spans="1:10" ht="16.5">
       <c r="A7" s="7" t="s">
@@ -17230,9 +17244,9 @@
       <c r="E7" s="189"/>
       <c r="F7" s="189"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="186"/>
-      <c r="I7" s="186"/>
-      <c r="J7" s="186"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="188"/>
     </row>
     <row r="8" spans="1:10" ht="16.5">
       <c r="A8" s="7" t="s">
@@ -17359,8 +17373,8 @@
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="186"/>
-      <c r="F14" s="186"/>
+      <c r="E14" s="188"/>
+      <c r="F14" s="188"/>
       <c r="G14" s="7" t="s">
         <v>179</v>
       </c>
@@ -17423,18 +17437,18 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="16.5">
-      <c r="A18" s="190" t="s">
+      <c r="A18" s="187" t="s">
         <v>105</v>
       </c>
-      <c r="B18" s="190"/>
-      <c r="C18" s="190"/>
-      <c r="D18" s="190"/>
-      <c r="E18" s="190"/>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
-      <c r="H18" s="190"/>
-      <c r="I18" s="190"/>
-      <c r="J18" s="190"/>
+      <c r="B18" s="187"/>
+      <c r="C18" s="187"/>
+      <c r="D18" s="187"/>
+      <c r="E18" s="187"/>
+      <c r="F18" s="187"/>
+      <c r="G18" s="187"/>
+      <c r="H18" s="187"/>
+      <c r="I18" s="187"/>
+      <c r="J18" s="187"/>
     </row>
     <row r="19" spans="1:10" ht="16.5">
       <c r="A19" s="10" t="s">
@@ -17464,9 +17478,9 @@
       <c r="E20" s="189"/>
       <c r="F20" s="189"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="186"/>
-      <c r="I20" s="186"/>
-      <c r="J20" s="186"/>
+      <c r="H20" s="188"/>
+      <c r="I20" s="188"/>
+      <c r="J20" s="188"/>
     </row>
     <row r="21" spans="1:10" ht="16.5">
       <c r="A21" s="10" t="s">
@@ -17484,9 +17498,9 @@
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="186"/>
-      <c r="I21" s="186"/>
-      <c r="J21" s="186"/>
+      <c r="H21" s="188"/>
+      <c r="I21" s="188"/>
+      <c r="J21" s="188"/>
     </row>
     <row r="22" spans="1:10" ht="16.5">
       <c r="A22" s="10" t="s">
@@ -17524,9 +17538,9 @@
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="186"/>
-      <c r="I23" s="186"/>
-      <c r="J23" s="186"/>
+      <c r="H23" s="188"/>
+      <c r="I23" s="188"/>
+      <c r="J23" s="188"/>
     </row>
     <row r="24" spans="1:10" ht="16.5">
       <c r="A24" s="10" t="s">
@@ -17544,9 +17558,9 @@
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="186"/>
-      <c r="I24" s="186"/>
-      <c r="J24" s="186"/>
+      <c r="H24" s="188"/>
+      <c r="I24" s="188"/>
+      <c r="J24" s="188"/>
     </row>
     <row r="25" spans="1:10" ht="16.5">
       <c r="A25" s="10" t="s">
@@ -17597,18 +17611,18 @@
       <c r="J26" s="189"/>
     </row>
     <row r="27" spans="1:10" ht="16.5">
-      <c r="A27" s="190" t="s">
+      <c r="A27" s="187" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="190"/>
-      <c r="C27" s="190"/>
-      <c r="D27" s="190"/>
-      <c r="E27" s="190"/>
-      <c r="F27" s="190"/>
-      <c r="G27" s="190"/>
-      <c r="H27" s="190"/>
-      <c r="I27" s="190"/>
-      <c r="J27" s="190"/>
+      <c r="B27" s="187"/>
+      <c r="C27" s="187"/>
+      <c r="D27" s="187"/>
+      <c r="E27" s="187"/>
+      <c r="F27" s="187"/>
+      <c r="G27" s="187"/>
+      <c r="H27" s="187"/>
+      <c r="I27" s="187"/>
+      <c r="J27" s="187"/>
     </row>
     <row r="28" spans="1:10" ht="16.5">
       <c r="A28" s="10" t="s">
@@ -17622,9 +17636,9 @@
       <c r="E28" s="189"/>
       <c r="F28" s="189"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="186"/>
-      <c r="I28" s="186"/>
-      <c r="J28" s="186"/>
+      <c r="H28" s="188"/>
+      <c r="I28" s="188"/>
+      <c r="J28" s="188"/>
     </row>
     <row r="29" spans="1:10" ht="16.5">
       <c r="A29" s="10" t="s">
@@ -17646,17 +17660,17 @@
       <c r="A30" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="187" t="s">
+      <c r="B30" s="190" t="s">
         <v>219</v>
       </c>
-      <c r="C30" s="187"/>
-      <c r="D30" s="187"/>
-      <c r="E30" s="187"/>
-      <c r="F30" s="187"/>
-      <c r="G30" s="187"/>
-      <c r="H30" s="187"/>
-      <c r="I30" s="187"/>
-      <c r="J30" s="187"/>
+      <c r="C30" s="190"/>
+      <c r="D30" s="190"/>
+      <c r="E30" s="190"/>
+      <c r="F30" s="190"/>
+      <c r="G30" s="190"/>
+      <c r="H30" s="190"/>
+      <c r="I30" s="190"/>
+      <c r="J30" s="190"/>
     </row>
     <row r="31" spans="1:10" ht="16.5">
       <c r="A31" s="10" t="s">
@@ -17678,17 +17692,17 @@
       <c r="A32" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="187" t="s">
+      <c r="B32" s="190" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="187"/>
-      <c r="D32" s="187"/>
-      <c r="E32" s="187"/>
-      <c r="F32" s="187"/>
-      <c r="G32" s="187"/>
-      <c r="H32" s="187"/>
-      <c r="I32" s="187"/>
-      <c r="J32" s="187"/>
+      <c r="C32" s="190"/>
+      <c r="D32" s="190"/>
+      <c r="E32" s="190"/>
+      <c r="F32" s="190"/>
+      <c r="G32" s="190"/>
+      <c r="H32" s="190"/>
+      <c r="I32" s="190"/>
+      <c r="J32" s="190"/>
     </row>
     <row r="33" spans="1:10" ht="16.5">
       <c r="A33" s="10" t="s">
@@ -17710,17 +17724,17 @@
       <c r="A34" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B34" s="187" t="s">
+      <c r="B34" s="190" t="s">
         <v>220</v>
       </c>
-      <c r="C34" s="187"/>
-      <c r="D34" s="187"/>
-      <c r="E34" s="187"/>
-      <c r="F34" s="187"/>
-      <c r="G34" s="187"/>
-      <c r="H34" s="187"/>
-      <c r="I34" s="187"/>
-      <c r="J34" s="187"/>
+      <c r="C34" s="190"/>
+      <c r="D34" s="190"/>
+      <c r="E34" s="190"/>
+      <c r="F34" s="190"/>
+      <c r="G34" s="190"/>
+      <c r="H34" s="190"/>
+      <c r="I34" s="190"/>
+      <c r="J34" s="190"/>
     </row>
     <row r="35" spans="1:10" ht="16.5">
       <c r="A35" s="10" t="s">
@@ -17734,23 +17748,23 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="186"/>
-      <c r="I35" s="186"/>
-      <c r="J35" s="186"/>
+      <c r="H35" s="188"/>
+      <c r="I35" s="188"/>
+      <c r="J35" s="188"/>
     </row>
     <row r="36" spans="1:10" ht="16.5">
-      <c r="A36" s="190" t="s">
+      <c r="A36" s="187" t="s">
         <v>107</v>
       </c>
-      <c r="B36" s="190"/>
-      <c r="C36" s="190"/>
-      <c r="D36" s="190"/>
-      <c r="E36" s="190"/>
-      <c r="F36" s="190"/>
-      <c r="G36" s="190"/>
-      <c r="H36" s="190"/>
-      <c r="I36" s="190"/>
-      <c r="J36" s="190"/>
+      <c r="B36" s="187"/>
+      <c r="C36" s="187"/>
+      <c r="D36" s="187"/>
+      <c r="E36" s="187"/>
+      <c r="F36" s="187"/>
+      <c r="G36" s="187"/>
+      <c r="H36" s="187"/>
+      <c r="I36" s="187"/>
+      <c r="J36" s="187"/>
     </row>
     <row r="37" spans="1:10" ht="16.5">
       <c r="A37" s="10" t="s">
@@ -17764,9 +17778,9 @@
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
-      <c r="H37" s="186"/>
-      <c r="I37" s="186"/>
-      <c r="J37" s="186"/>
+      <c r="H37" s="188"/>
+      <c r="I37" s="188"/>
+      <c r="J37" s="188"/>
     </row>
     <row r="38" spans="1:10" ht="16.5">
       <c r="A38" s="10" t="s">
@@ -17872,9 +17886,9 @@
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="11"/>
-      <c r="H42" s="188"/>
-      <c r="I42" s="188"/>
-      <c r="J42" s="188"/>
+      <c r="H42" s="191"/>
+      <c r="I42" s="191"/>
+      <c r="J42" s="191"/>
     </row>
     <row r="43" spans="1:10">
       <c r="B43" s="4"/>
@@ -17899,6 +17913,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H37:J37"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="A27:J27"/>
@@ -17915,32 +17955,6 @@
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="B33:J33"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B32:J32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -18782,7 +18796,7 @@
       <c r="E5" s="159"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="191" t="s">
+      <c r="A6" s="194" t="s">
         <v>1814</v>
       </c>
       <c r="B6" s="166" t="s">
@@ -18794,10 +18808,10 @@
       <c r="D6" s="157" t="s">
         <v>1638</v>
       </c>
-      <c r="E6" s="192"/>
+      <c r="E6" s="214"/>
     </row>
     <row r="7" spans="1:5" ht="49.5">
-      <c r="A7" s="191" t="str">
+      <c r="A7" s="194" t="str">
         <f t="shared" ref="A7:A12" si="0">A6</f>
         <v>控件</v>
       </c>
@@ -18810,10 +18824,10 @@
       <c r="D7" s="157" t="s">
         <v>1649</v>
       </c>
-      <c r="E7" s="193"/>
+      <c r="E7" s="215"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="191" t="str">
+      <c r="A8" s="194" t="str">
         <f t="shared" si="0"/>
         <v>控件</v>
       </c>
@@ -18826,10 +18840,10 @@
       <c r="D8" s="168" t="s">
         <v>1776</v>
       </c>
-      <c r="E8" s="193"/>
+      <c r="E8" s="215"/>
     </row>
     <row r="9" spans="1:5" ht="49.5">
-      <c r="A9" s="191" t="str">
+      <c r="A9" s="194" t="str">
         <f t="shared" si="0"/>
         <v>控件</v>
       </c>
@@ -18842,10 +18856,10 @@
       <c r="D9" s="168" t="s">
         <v>1803</v>
       </c>
-      <c r="E9" s="193"/>
+      <c r="E9" s="215"/>
     </row>
     <row r="10" spans="1:5" ht="66">
-      <c r="A10" s="191" t="str">
+      <c r="A10" s="194" t="str">
         <f t="shared" si="0"/>
         <v>控件</v>
       </c>
@@ -18858,10 +18872,10 @@
       <c r="D10" s="168" t="s">
         <v>1817</v>
       </c>
-      <c r="E10" s="193"/>
+      <c r="E10" s="215"/>
     </row>
     <row r="11" spans="1:5" ht="66">
-      <c r="A11" s="191" t="str">
+      <c r="A11" s="194" t="str">
         <f t="shared" si="0"/>
         <v>控件</v>
       </c>
@@ -18874,10 +18888,10 @@
       <c r="D11" s="168" t="s">
         <v>1835</v>
       </c>
-      <c r="E11" s="193"/>
+      <c r="E11" s="215"/>
     </row>
     <row r="12" spans="1:5" ht="49.5">
-      <c r="A12" s="191" t="str">
+      <c r="A12" s="194" t="str">
         <f t="shared" si="0"/>
         <v>控件</v>
       </c>
@@ -18890,10 +18904,10 @@
       <c r="D12" s="157" t="s">
         <v>1643</v>
       </c>
-      <c r="E12" s="193"/>
+      <c r="E12" s="215"/>
     </row>
     <row r="13" spans="1:5" ht="33">
-      <c r="A13" s="191"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="166" t="s">
         <v>1918</v>
       </c>
@@ -18903,10 +18917,10 @@
       <c r="D13" s="157" t="s">
         <v>1920</v>
       </c>
-      <c r="E13" s="193"/>
+      <c r="E13" s="215"/>
     </row>
     <row r="14" spans="1:5" ht="115.5">
-      <c r="A14" s="191"/>
+      <c r="A14" s="194"/>
       <c r="B14" s="166" t="s">
         <v>1932</v>
       </c>
@@ -18916,10 +18930,10 @@
       <c r="D14" s="157" t="s">
         <v>1934</v>
       </c>
-      <c r="E14" s="193"/>
+      <c r="E14" s="215"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="191"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="169" t="s">
         <v>1969</v>
       </c>
@@ -18929,10 +18943,10 @@
       <c r="D15" s="157" t="s">
         <v>1971</v>
       </c>
-      <c r="E15" s="193"/>
+      <c r="E15" s="215"/>
     </row>
     <row r="16" spans="1:5" ht="82.5">
-      <c r="A16" s="191"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="169" t="s">
         <v>1981</v>
       </c>
@@ -18942,11 +18956,11 @@
       <c r="D16" s="157" t="s">
         <v>1982</v>
       </c>
-      <c r="E16" s="193"/>
+      <c r="E16" s="215"/>
     </row>
     <row r="17" spans="1:5" ht="33">
-      <c r="A17" s="191"/>
-      <c r="B17" s="205" t="s">
+      <c r="A17" s="194"/>
+      <c r="B17" s="198" t="s">
         <v>2011</v>
       </c>
       <c r="C17" s="157" t="s">
@@ -18955,22 +18969,22 @@
       <c r="D17" s="157" t="s">
         <v>2013</v>
       </c>
-      <c r="E17" s="193"/>
+      <c r="E17" s="215"/>
     </row>
     <row r="18" spans="1:5" ht="115.5">
-      <c r="A18" s="191"/>
-      <c r="B18" s="206"/>
+      <c r="A18" s="194"/>
+      <c r="B18" s="199"/>
       <c r="C18" s="157" t="s">
         <v>2014</v>
       </c>
       <c r="D18" s="157" t="s">
         <v>2015</v>
       </c>
-      <c r="E18" s="193"/>
+      <c r="E18" s="215"/>
     </row>
     <row r="19" spans="1:5" ht="33">
-      <c r="A19" s="191"/>
-      <c r="B19" s="205" t="s">
+      <c r="A19" s="194"/>
+      <c r="B19" s="198" t="s">
         <v>2016</v>
       </c>
       <c r="C19" s="157" t="s">
@@ -18979,21 +18993,21 @@
       <c r="D19" s="157" t="s">
         <v>2018</v>
       </c>
-      <c r="E19" s="193"/>
+      <c r="E19" s="215"/>
     </row>
     <row r="20" spans="1:5" ht="66">
-      <c r="A20" s="191"/>
-      <c r="B20" s="206"/>
+      <c r="A20" s="194"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="157" t="s">
         <v>2161</v>
       </c>
       <c r="D20" s="157" t="s">
         <v>2160</v>
       </c>
-      <c r="E20" s="193"/>
+      <c r="E20" s="215"/>
     </row>
     <row r="21" spans="1:5" ht="66">
-      <c r="A21" s="191"/>
+      <c r="A21" s="194"/>
       <c r="B21" s="183" t="s">
         <v>2019</v>
       </c>
@@ -19003,10 +19017,10 @@
       <c r="D21" s="157" t="s">
         <v>2020</v>
       </c>
-      <c r="E21" s="193"/>
+      <c r="E21" s="215"/>
     </row>
     <row r="22" spans="1:5" ht="115.5">
-      <c r="A22" s="191"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="183" t="s">
         <v>2034</v>
       </c>
@@ -19016,10 +19030,10 @@
       <c r="D22" s="157" t="s">
         <v>2035</v>
       </c>
-      <c r="E22" s="193"/>
+      <c r="E22" s="215"/>
     </row>
     <row r="23" spans="1:5" ht="82.5">
-      <c r="A23" s="191"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="183" t="s">
         <v>2090</v>
       </c>
@@ -19029,10 +19043,10 @@
       <c r="D23" s="157" t="s">
         <v>2092</v>
       </c>
-      <c r="E23" s="193"/>
+      <c r="E23" s="215"/>
     </row>
     <row r="24" spans="1:5" ht="165">
-      <c r="A24" s="191"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="183" t="s">
         <v>2203</v>
       </c>
@@ -19042,10 +19056,10 @@
       <c r="D24" s="157" t="s">
         <v>2205</v>
       </c>
-      <c r="E24" s="193"/>
+      <c r="E24" s="215"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="191"/>
+      <c r="A25" s="194"/>
       <c r="B25" s="182" t="s">
         <v>1896</v>
       </c>
@@ -19055,10 +19069,10 @@
       <c r="D25" s="157" t="s">
         <v>1898</v>
       </c>
-      <c r="E25" s="193"/>
+      <c r="E25" s="215"/>
     </row>
     <row r="26" spans="1:5" ht="280.5">
-      <c r="A26" s="191"/>
+      <c r="A26" s="194"/>
       <c r="B26" s="182" t="s">
         <v>2208</v>
       </c>
@@ -19068,10 +19082,10 @@
       <c r="D26" s="157" t="s">
         <v>2210</v>
       </c>
-      <c r="E26" s="193"/>
+      <c r="E26" s="215"/>
     </row>
     <row r="27" spans="1:5" ht="165">
-      <c r="A27" s="191"/>
+      <c r="A27" s="194"/>
       <c r="B27" s="182" t="s">
         <v>2211</v>
       </c>
@@ -19081,10 +19095,10 @@
       <c r="D27" s="157" t="s">
         <v>2212</v>
       </c>
-      <c r="E27" s="193"/>
+      <c r="E27" s="215"/>
     </row>
     <row r="28" spans="1:5" ht="33">
-      <c r="A28" s="191"/>
+      <c r="A28" s="194"/>
       <c r="B28" s="182" t="s">
         <v>2215</v>
       </c>
@@ -19094,10 +19108,10 @@
       <c r="D28" s="157" t="s">
         <v>2216</v>
       </c>
-      <c r="E28" s="193"/>
+      <c r="E28" s="215"/>
     </row>
     <row r="29" spans="1:5" ht="198">
-      <c r="A29" s="191"/>
+      <c r="A29" s="194"/>
       <c r="B29" s="182" t="s">
         <v>2218</v>
       </c>
@@ -19107,10 +19121,10 @@
       <c r="D29" s="157" t="s">
         <v>2219</v>
       </c>
-      <c r="E29" s="193"/>
+      <c r="E29" s="215"/>
     </row>
     <row r="30" spans="1:5" ht="264">
-      <c r="A30" s="191" t="str">
+      <c r="A30" s="194" t="str">
         <f>A12</f>
         <v>控件</v>
       </c>
@@ -19123,7 +19137,7 @@
       <c r="D30" s="157" t="s">
         <v>2207</v>
       </c>
-      <c r="E30" s="194"/>
+      <c r="E30" s="216"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="166" t="s">
@@ -19165,7 +19179,7 @@
       <c r="E33" s="158"/>
     </row>
     <row r="34" spans="1:5" ht="165">
-      <c r="A34" s="191" t="s">
+      <c r="A34" s="194" t="s">
         <v>1771</v>
       </c>
       <c r="B34" s="170" t="s">
@@ -19177,10 +19191,10 @@
       <c r="D34" s="168" t="s">
         <v>1772</v>
       </c>
-      <c r="E34" s="192"/>
+      <c r="E34" s="214"/>
     </row>
     <row r="35" spans="1:5" ht="66">
-      <c r="A35" s="191" t="str">
+      <c r="A35" s="194" t="str">
         <f t="shared" ref="A35" si="1">A34</f>
         <v>textvariable</v>
       </c>
@@ -19193,10 +19207,10 @@
       <c r="D35" s="168" t="s">
         <v>1778</v>
       </c>
-      <c r="E35" s="193"/>
+      <c r="E35" s="215"/>
     </row>
     <row r="36" spans="1:5" ht="66">
-      <c r="A36" s="191"/>
+      <c r="A36" s="194"/>
       <c r="B36" s="170" t="s">
         <v>1969</v>
       </c>
@@ -19206,10 +19220,10 @@
       <c r="D36" s="168" t="s">
         <v>1977</v>
       </c>
-      <c r="E36" s="193"/>
+      <c r="E36" s="215"/>
     </row>
     <row r="37" spans="1:5" ht="49.5">
-      <c r="A37" s="191"/>
+      <c r="A37" s="194"/>
       <c r="B37" s="170" t="s">
         <v>2046</v>
       </c>
@@ -19219,10 +19233,10 @@
       <c r="D37" s="168" t="s">
         <v>2048</v>
       </c>
-      <c r="E37" s="193"/>
+      <c r="E37" s="215"/>
     </row>
     <row r="38" spans="1:5" ht="49.5">
-      <c r="A38" s="191" t="str">
+      <c r="A38" s="194" t="str">
         <f>A35</f>
         <v>textvariable</v>
       </c>
@@ -19235,10 +19249,10 @@
       <c r="D38" s="168" t="s">
         <v>1907</v>
       </c>
-      <c r="E38" s="194"/>
+      <c r="E38" s="216"/>
     </row>
     <row r="39" spans="1:5" ht="82.5">
-      <c r="A39" s="214" t="s">
+      <c r="A39" s="208" t="s">
         <v>1808</v>
       </c>
       <c r="B39" s="157" t="s">
@@ -19250,10 +19264,10 @@
       <c r="D39" s="168" t="s">
         <v>1810</v>
       </c>
-      <c r="E39" s="195"/>
+      <c r="E39" s="217"/>
     </row>
     <row r="40" spans="1:5" ht="66">
-      <c r="A40" s="214" t="str">
+      <c r="A40" s="208" t="str">
         <f>A39</f>
         <v>variable</v>
       </c>
@@ -19266,10 +19280,10 @@
       <c r="D40" s="168" t="s">
         <v>1821</v>
       </c>
-      <c r="E40" s="195"/>
+      <c r="E40" s="217"/>
     </row>
     <row r="41" spans="1:5" ht="66">
-      <c r="A41" s="214" t="s">
+      <c r="A41" s="208" t="s">
         <v>1828</v>
       </c>
       <c r="B41" s="157" t="s">
@@ -19281,10 +19295,10 @@
       <c r="D41" s="168" t="s">
         <v>1829</v>
       </c>
-      <c r="E41" s="212"/>
+      <c r="E41" s="206"/>
     </row>
     <row r="42" spans="1:5" ht="66">
-      <c r="A42" s="214" t="str">
+      <c r="A42" s="208" t="str">
         <f>A41</f>
         <v>value</v>
       </c>
@@ -19297,7 +19311,7 @@
       <c r="D42" s="168" t="s">
         <v>1903</v>
       </c>
-      <c r="E42" s="213"/>
+      <c r="E42" s="207"/>
     </row>
     <row r="43" spans="1:5" ht="99">
       <c r="A43" s="171" t="s">
@@ -19315,7 +19329,7 @@
       <c r="E43" s="160"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="191" t="s">
+      <c r="A44" s="194" t="s">
         <v>1654</v>
       </c>
       <c r="B44" s="170" t="s">
@@ -19327,10 +19341,10 @@
       <c r="D44" s="157" t="s">
         <v>1822</v>
       </c>
-      <c r="E44" s="196"/>
+      <c r="E44" s="204"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="191" t="str">
+      <c r="A45" s="194" t="str">
         <f t="shared" ref="A45:A54" si="2">A44</f>
         <v>bitmap</v>
       </c>
@@ -19341,10 +19355,10 @@
       <c r="D45" s="157" t="s">
         <v>1704</v>
       </c>
-      <c r="E45" s="196"/>
+      <c r="E45" s="204"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="191" t="str">
+      <c r="A46" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19355,10 +19369,10 @@
       <c r="D46" s="157" t="s">
         <v>1705</v>
       </c>
-      <c r="E46" s="196"/>
+      <c r="E46" s="204"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="191" t="str">
+      <c r="A47" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19369,10 +19383,10 @@
       <c r="D47" s="157" t="s">
         <v>1706</v>
       </c>
-      <c r="E47" s="196"/>
+      <c r="E47" s="204"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="191" t="str">
+      <c r="A48" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19383,10 +19397,10 @@
       <c r="D48" s="157" t="s">
         <v>1707</v>
       </c>
-      <c r="E48" s="196"/>
+      <c r="E48" s="204"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="191" t="str">
+      <c r="A49" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19397,10 +19411,10 @@
       <c r="D49" s="157" t="s">
         <v>1708</v>
       </c>
-      <c r="E49" s="196"/>
+      <c r="E49" s="204"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="191" t="str">
+      <c r="A50" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19411,10 +19425,10 @@
       <c r="D50" s="157" t="s">
         <v>1709</v>
       </c>
-      <c r="E50" s="196"/>
+      <c r="E50" s="204"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="191" t="str">
+      <c r="A51" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19425,10 +19439,10 @@
       <c r="D51" s="157" t="s">
         <v>1710</v>
       </c>
-      <c r="E51" s="196"/>
+      <c r="E51" s="204"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="191" t="str">
+      <c r="A52" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19439,10 +19453,10 @@
       <c r="D52" s="157" t="s">
         <v>1711</v>
       </c>
-      <c r="E52" s="196"/>
+      <c r="E52" s="204"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="191" t="str">
+      <c r="A53" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19453,10 +19467,10 @@
       <c r="D53" s="157" t="s">
         <v>1712</v>
       </c>
-      <c r="E53" s="196"/>
+      <c r="E53" s="204"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="191" t="str">
+      <c r="A54" s="194" t="str">
         <f t="shared" si="2"/>
         <v>bitmap</v>
       </c>
@@ -19467,10 +19481,10 @@
       <c r="D54" s="157" t="s">
         <v>1713</v>
       </c>
-      <c r="E54" s="196"/>
+      <c r="E54" s="204"/>
     </row>
     <row r="55" spans="1:5" ht="33">
-      <c r="A55" s="191" t="s">
+      <c r="A55" s="194" t="s">
         <v>1686</v>
       </c>
       <c r="B55" s="170" t="s">
@@ -19482,10 +19496,10 @@
       <c r="D55" s="157" t="s">
         <v>1688</v>
       </c>
-      <c r="E55" s="196"/>
+      <c r="E55" s="204"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="191" t="str">
+      <c r="A56" s="194" t="str">
         <f t="shared" ref="A56:A60" si="3">A55</f>
         <v>compound</v>
       </c>
@@ -19494,10 +19508,10 @@
         <v>1690</v>
       </c>
       <c r="D56" s="157"/>
-      <c r="E56" s="196"/>
+      <c r="E56" s="204"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="191" t="str">
+      <c r="A57" s="194" t="str">
         <f t="shared" si="3"/>
         <v>compound</v>
       </c>
@@ -19506,10 +19520,10 @@
         <v>1691</v>
       </c>
       <c r="D57" s="157"/>
-      <c r="E57" s="196"/>
+      <c r="E57" s="204"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="191" t="str">
+      <c r="A58" s="194" t="str">
         <f t="shared" si="3"/>
         <v>compound</v>
       </c>
@@ -19518,10 +19532,10 @@
         <v>1692</v>
       </c>
       <c r="D58" s="157"/>
-      <c r="E58" s="196"/>
+      <c r="E58" s="204"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="191" t="str">
+      <c r="A59" s="194" t="str">
         <f t="shared" si="3"/>
         <v>compound</v>
       </c>
@@ -19530,10 +19544,10 @@
         <v>1693</v>
       </c>
       <c r="D59" s="157"/>
-      <c r="E59" s="196"/>
+      <c r="E59" s="204"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="191" t="str">
+      <c r="A60" s="194" t="str">
         <f t="shared" si="3"/>
         <v>compound</v>
       </c>
@@ -19542,10 +19556,10 @@
         <v>1823</v>
       </c>
       <c r="D60" s="157"/>
-      <c r="E60" s="196"/>
+      <c r="E60" s="204"/>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="191" t="s">
+      <c r="A61" s="194" t="s">
         <v>1670</v>
       </c>
       <c r="B61" s="170" t="s">
@@ -19555,10 +19569,10 @@
         <v>1671</v>
       </c>
       <c r="D61" s="157"/>
-      <c r="E61" s="196"/>
+      <c r="E61" s="204"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="191" t="str">
+      <c r="A62" s="194" t="str">
         <f t="shared" ref="A62:A74" si="4">A61</f>
         <v>fg/bg</v>
       </c>
@@ -19567,10 +19581,10 @@
         <v>1677</v>
       </c>
       <c r="D62" s="157"/>
-      <c r="E62" s="196"/>
+      <c r="E62" s="204"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="191" t="str">
+      <c r="A63" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19581,10 +19595,10 @@
       <c r="D63" s="157" t="s">
         <v>1714</v>
       </c>
-      <c r="E63" s="196"/>
+      <c r="E63" s="204"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="191" t="str">
+      <c r="A64" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19595,10 +19609,10 @@
       <c r="D64" s="157" t="s">
         <v>1715</v>
       </c>
-      <c r="E64" s="196"/>
+      <c r="E64" s="204"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="191" t="str">
+      <c r="A65" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19609,10 +19623,10 @@
       <c r="D65" s="157" t="s">
         <v>1716</v>
       </c>
-      <c r="E65" s="196"/>
+      <c r="E65" s="204"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="191" t="str">
+      <c r="A66" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19623,10 +19637,10 @@
       <c r="D66" s="157" t="s">
         <v>1717</v>
       </c>
-      <c r="E66" s="196"/>
+      <c r="E66" s="204"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="191" t="str">
+      <c r="A67" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19637,10 +19651,10 @@
       <c r="D67" s="157" t="s">
         <v>1718</v>
       </c>
-      <c r="E67" s="196"/>
+      <c r="E67" s="204"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="191" t="str">
+      <c r="A68" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19649,10 +19663,10 @@
         <v>1678</v>
       </c>
       <c r="D68" s="157"/>
-      <c r="E68" s="196"/>
+      <c r="E68" s="204"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="191" t="str">
+      <c r="A69" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19661,10 +19675,10 @@
         <v>1679</v>
       </c>
       <c r="D69" s="157"/>
-      <c r="E69" s="196"/>
+      <c r="E69" s="204"/>
     </row>
     <row r="70" spans="1:5" ht="33">
-      <c r="A70" s="191" t="str">
+      <c r="A70" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19673,10 +19687,10 @@
         <v>1680</v>
       </c>
       <c r="D70" s="157"/>
-      <c r="E70" s="196"/>
+      <c r="E70" s="204"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="191" t="str">
+      <c r="A71" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19685,10 +19699,10 @@
         <v>1681</v>
       </c>
       <c r="D71" s="157"/>
-      <c r="E71" s="196"/>
+      <c r="E71" s="204"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="191" t="str">
+      <c r="A72" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19697,10 +19711,10 @@
         <v>1682</v>
       </c>
       <c r="D72" s="157"/>
-      <c r="E72" s="196"/>
+      <c r="E72" s="204"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="191" t="str">
+      <c r="A73" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19709,10 +19723,10 @@
         <v>1683</v>
       </c>
       <c r="D73" s="173"/>
-      <c r="E73" s="196"/>
+      <c r="E73" s="204"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="191" t="str">
+      <c r="A74" s="194" t="str">
         <f t="shared" si="4"/>
         <v>fg/bg</v>
       </c>
@@ -19721,7 +19735,7 @@
         <v>1684</v>
       </c>
       <c r="D74" s="173"/>
-      <c r="E74" s="196"/>
+      <c r="E74" s="204"/>
     </row>
     <row r="75" spans="1:5" ht="33">
       <c r="A75" s="166" t="s">
@@ -19780,7 +19794,7 @@
       <c r="E78" s="158"/>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="191" t="s">
+      <c r="A79" s="194" t="s">
         <v>1698</v>
       </c>
       <c r="B79" s="170" t="s">
@@ -19790,10 +19804,10 @@
         <v>1719</v>
       </c>
       <c r="D79" s="157"/>
-      <c r="E79" s="196"/>
+      <c r="E79" s="204"/>
     </row>
     <row r="80" spans="1:5" ht="33">
-      <c r="A80" s="191" t="str">
+      <c r="A80" s="194" t="str">
         <f t="shared" ref="A80:A81" si="5">A79</f>
         <v>justify</v>
       </c>
@@ -19804,10 +19818,10 @@
       <c r="D80" s="157" t="s">
         <v>1721</v>
       </c>
-      <c r="E80" s="196"/>
+      <c r="E80" s="204"/>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="191" t="str">
+      <c r="A81" s="194" t="str">
         <f t="shared" si="5"/>
         <v>justify</v>
       </c>
@@ -19816,7 +19830,7 @@
         <v>1703</v>
       </c>
       <c r="D81" s="157"/>
-      <c r="E81" s="196"/>
+      <c r="E81" s="204"/>
     </row>
     <row r="82" spans="1:5" ht="33">
       <c r="A82" s="169"/>
@@ -19832,7 +19846,7 @@
       <c r="E82" s="161"/>
     </row>
     <row r="83" spans="1:5" ht="33">
-      <c r="A83" s="191" t="s">
+      <c r="A83" s="194" t="s">
         <v>1699</v>
       </c>
       <c r="B83" s="170" t="s">
@@ -19842,10 +19856,10 @@
         <v>1700</v>
       </c>
       <c r="D83" s="157"/>
-      <c r="E83" s="196"/>
+      <c r="E83" s="204"/>
     </row>
     <row r="84" spans="1:5" ht="66">
-      <c r="A84" s="191" t="str">
+      <c r="A84" s="194" t="str">
         <f>A83</f>
         <v>ahchor</v>
       </c>
@@ -19856,10 +19870,10 @@
       <c r="D84" s="157" t="s">
         <v>1722</v>
       </c>
-      <c r="E84" s="196"/>
+      <c r="E84" s="204"/>
     </row>
     <row r="85" spans="1:5" s="91" customFormat="1" ht="33">
-      <c r="A85" s="215" t="s">
+      <c r="A85" s="195" t="s">
         <v>1763</v>
       </c>
       <c r="B85" s="174" t="s">
@@ -19871,10 +19885,10 @@
       <c r="D85" s="174" t="s">
         <v>1764</v>
       </c>
-      <c r="E85" s="211"/>
+      <c r="E85" s="205"/>
     </row>
     <row r="86" spans="1:5" s="91" customFormat="1">
-      <c r="A86" s="215" t="str">
+      <c r="A86" s="195" t="str">
         <f t="shared" ref="A86:A87" si="6">A85</f>
         <v>StringVar</v>
       </c>
@@ -19887,10 +19901,10 @@
       <c r="D86" s="174" t="s">
         <v>1765</v>
       </c>
-      <c r="E86" s="211"/>
+      <c r="E86" s="205"/>
     </row>
     <row r="87" spans="1:5" s="91" customFormat="1">
-      <c r="A87" s="215" t="str">
+      <c r="A87" s="195" t="str">
         <f t="shared" si="6"/>
         <v>StringVar</v>
       </c>
@@ -19903,10 +19917,10 @@
       <c r="D87" s="174" t="s">
         <v>1769</v>
       </c>
-      <c r="E87" s="211"/>
+      <c r="E87" s="205"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="191" t="s">
+      <c r="A88" s="194" t="s">
         <v>1868</v>
       </c>
       <c r="B88" s="174" t="s">
@@ -19918,10 +19932,10 @@
       <c r="D88" s="157" t="s">
         <v>1870</v>
       </c>
-      <c r="E88" s="196"/>
+      <c r="E88" s="204"/>
     </row>
     <row r="89" spans="1:5" s="91" customFormat="1">
-      <c r="A89" s="191" t="str">
+      <c r="A89" s="194" t="str">
         <f t="shared" ref="A89:A90" si="7">A88</f>
         <v>IntVar</v>
       </c>
@@ -19934,10 +19948,10 @@
       <c r="D89" s="174" t="s">
         <v>1765</v>
       </c>
-      <c r="E89" s="196"/>
+      <c r="E89" s="204"/>
     </row>
     <row r="90" spans="1:5" s="91" customFormat="1">
-      <c r="A90" s="191" t="str">
+      <c r="A90" s="194" t="str">
         <f t="shared" si="7"/>
         <v>IntVar</v>
       </c>
@@ -19950,10 +19964,10 @@
       <c r="D90" s="174" t="s">
         <v>1871</v>
       </c>
-      <c r="E90" s="196"/>
+      <c r="E90" s="204"/>
     </row>
     <row r="91" spans="1:5" ht="33">
-      <c r="A91" s="216" t="s">
+      <c r="A91" s="196" t="s">
         <v>1728</v>
       </c>
       <c r="B91" s="170" t="s">
@@ -19965,10 +19979,10 @@
       <c r="D91" s="168" t="s">
         <v>1729</v>
       </c>
-      <c r="E91" s="196"/>
+      <c r="E91" s="204"/>
     </row>
     <row r="92" spans="1:5" ht="33">
-      <c r="A92" s="216" t="str">
+      <c r="A92" s="196" t="str">
         <f t="shared" ref="A92" si="8">A91</f>
         <v>command</v>
       </c>
@@ -19981,10 +19995,10 @@
       <c r="D92" s="168" t="s">
         <v>1806</v>
       </c>
-      <c r="E92" s="196"/>
+      <c r="E92" s="204"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="216"/>
+      <c r="A93" s="196"/>
       <c r="B93" s="170" t="s">
         <v>1918</v>
       </c>
@@ -19994,10 +20008,10 @@
       <c r="D93" s="168" t="s">
         <v>1924</v>
       </c>
-      <c r="E93" s="196"/>
+      <c r="E93" s="204"/>
     </row>
     <row r="94" spans="1:5" ht="49.5">
-      <c r="A94" s="216" t="str">
+      <c r="A94" s="196" t="str">
         <f>A91</f>
         <v>command</v>
       </c>
@@ -20010,10 +20024,10 @@
       <c r="D94" s="168" t="s">
         <v>1908</v>
       </c>
-      <c r="E94" s="196"/>
+      <c r="E94" s="204"/>
     </row>
     <row r="95" spans="1:5" ht="82.5">
-      <c r="A95" s="216"/>
+      <c r="A95" s="196"/>
       <c r="B95" s="170" t="s">
         <v>1981</v>
       </c>
@@ -20023,10 +20037,10 @@
       <c r="D95" s="168" t="s">
         <v>1984</v>
       </c>
-      <c r="E95" s="196"/>
+      <c r="E95" s="204"/>
     </row>
     <row r="96" spans="1:5" ht="115.5">
-      <c r="A96" s="216" t="str">
+      <c r="A96" s="196" t="str">
         <f>A92</f>
         <v>command</v>
       </c>
@@ -20039,7 +20053,7 @@
       <c r="D96" s="168" t="s">
         <v>1885</v>
       </c>
-      <c r="E96" s="196"/>
+      <c r="E96" s="204"/>
     </row>
     <row r="97" spans="1:5" ht="132">
       <c r="A97" s="180"/>
@@ -20120,7 +20134,7 @@
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="191" t="s">
+      <c r="A103" s="194" t="s">
         <v>1731</v>
       </c>
       <c r="B103" s="170" t="s">
@@ -20130,10 +20144,10 @@
         <v>1759</v>
       </c>
       <c r="D103" s="168"/>
-      <c r="E103" s="196"/>
+      <c r="E103" s="204"/>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="191" t="str">
+      <c r="A104" s="194" t="str">
         <f t="shared" ref="A104:A109" si="9">A103</f>
         <v>relief</v>
       </c>
@@ -20144,10 +20158,10 @@
       <c r="D104" s="168" t="s">
         <v>1738</v>
       </c>
-      <c r="E104" s="196"/>
+      <c r="E104" s="204"/>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="191" t="str">
+      <c r="A105" s="194" t="str">
         <f t="shared" si="9"/>
         <v>relief</v>
       </c>
@@ -20158,10 +20172,10 @@
       <c r="D105" s="168" t="s">
         <v>1739</v>
       </c>
-      <c r="E105" s="196"/>
+      <c r="E105" s="204"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="191" t="str">
+      <c r="A106" s="194" t="str">
         <f t="shared" si="9"/>
         <v>relief</v>
       </c>
@@ -20172,10 +20186,10 @@
       <c r="D106" s="168" t="s">
         <v>1740</v>
       </c>
-      <c r="E106" s="196"/>
+      <c r="E106" s="204"/>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="191" t="str">
+      <c r="A107" s="194" t="str">
         <f t="shared" si="9"/>
         <v>relief</v>
       </c>
@@ -20186,10 +20200,10 @@
       <c r="D107" s="168" t="s">
         <v>1741</v>
       </c>
-      <c r="E107" s="196"/>
+      <c r="E107" s="204"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="191" t="str">
+      <c r="A108" s="194" t="str">
         <f t="shared" si="9"/>
         <v>relief</v>
       </c>
@@ -20200,10 +20214,10 @@
       <c r="D108" s="168" t="s">
         <v>1742</v>
       </c>
-      <c r="E108" s="196"/>
+      <c r="E108" s="204"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="191" t="str">
+      <c r="A109" s="194" t="str">
         <f t="shared" si="9"/>
         <v>relief</v>
       </c>
@@ -20214,7 +20228,7 @@
       <c r="D109" s="168" t="s">
         <v>1743</v>
       </c>
-      <c r="E109" s="196"/>
+      <c r="E109" s="204"/>
     </row>
     <row r="110" spans="1:5" ht="33">
       <c r="A110" s="166" t="s">
@@ -20232,7 +20246,7 @@
       <c r="E110" s="158"/>
     </row>
     <row r="111" spans="1:5" ht="99">
-      <c r="A111" s="191" t="s">
+      <c r="A111" s="194" t="s">
         <v>1760</v>
       </c>
       <c r="B111" s="170" t="s">
@@ -20244,10 +20258,10 @@
       <c r="D111" s="168" t="s">
         <v>1761</v>
       </c>
-      <c r="E111" s="196"/>
+      <c r="E111" s="204"/>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="191" t="str">
+      <c r="A112" s="194" t="str">
         <f t="shared" ref="A112:A114" si="10">A111</f>
         <v>state</v>
       </c>
@@ -20258,10 +20272,10 @@
       <c r="D112" s="168" t="s">
         <v>1791</v>
       </c>
-      <c r="E112" s="196"/>
+      <c r="E112" s="204"/>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="191" t="str">
+      <c r="A113" s="194" t="str">
         <f t="shared" si="10"/>
         <v>state</v>
       </c>
@@ -20272,10 +20286,10 @@
       <c r="D113" s="168" t="s">
         <v>1792</v>
       </c>
-      <c r="E113" s="196"/>
+      <c r="E113" s="204"/>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="191" t="str">
+      <c r="A114" s="194" t="str">
         <f t="shared" si="10"/>
         <v>state</v>
       </c>
@@ -20286,7 +20300,7 @@
       <c r="D114" s="168" t="s">
         <v>1793</v>
       </c>
-      <c r="E114" s="196"/>
+      <c r="E114" s="204"/>
     </row>
     <row r="115" spans="1:5" ht="33">
       <c r="A115" s="166" t="s">
@@ -20332,59 +20346,59 @@
       <c r="E117" s="160"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="191" t="s">
+      <c r="A118" s="194" t="s">
         <v>1836</v>
       </c>
-      <c r="B118" s="191" t="s">
+      <c r="B118" s="194" t="s">
         <v>1837</v>
       </c>
       <c r="C118" s="157" t="s">
         <v>1839</v>
       </c>
       <c r="D118" s="157"/>
-      <c r="E118" s="197"/>
+      <c r="E118" s="209"/>
     </row>
     <row r="119" spans="1:5" ht="33">
-      <c r="A119" s="191" t="str">
+      <c r="A119" s="194" t="str">
         <f t="shared" ref="A119:A121" si="11">A118</f>
         <v>selectmode</v>
       </c>
-      <c r="B119" s="191"/>
+      <c r="B119" s="194"/>
       <c r="C119" s="157" t="s">
         <v>1840</v>
       </c>
       <c r="D119" s="157" t="s">
         <v>1841</v>
       </c>
-      <c r="E119" s="198"/>
+      <c r="E119" s="211"/>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="191" t="str">
+      <c r="A120" s="194" t="str">
         <f t="shared" si="11"/>
         <v>selectmode</v>
       </c>
-      <c r="B120" s="191"/>
+      <c r="B120" s="194"/>
       <c r="C120" s="157" t="s">
         <v>1842</v>
       </c>
       <c r="D120" s="157" t="s">
         <v>1838</v>
       </c>
-      <c r="E120" s="198"/>
+      <c r="E120" s="211"/>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="191" t="str">
+      <c r="A121" s="194" t="str">
         <f t="shared" si="11"/>
         <v>selectmode</v>
       </c>
-      <c r="B121" s="191"/>
+      <c r="B121" s="194"/>
       <c r="C121" s="157" t="s">
         <v>1844</v>
       </c>
       <c r="D121" s="157" t="s">
         <v>1843</v>
       </c>
-      <c r="E121" s="199"/>
+      <c r="E121" s="210"/>
     </row>
     <row r="122" spans="1:5" ht="49.5">
       <c r="A122" s="166" t="s">
@@ -20467,7 +20481,7 @@
       <c r="E127" s="181"/>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="191" t="s">
+      <c r="A128" s="194" t="s">
         <v>1859</v>
       </c>
       <c r="B128" s="157" t="s">
@@ -20479,10 +20493,10 @@
       <c r="D128" s="157" t="s">
         <v>1864</v>
       </c>
-      <c r="E128" s="200"/>
+      <c r="E128" s="212"/>
     </row>
     <row r="129" spans="1:5">
-      <c r="A129" s="191"/>
+      <c r="A129" s="194"/>
       <c r="B129" s="157" t="s">
         <v>1783</v>
       </c>
@@ -20492,10 +20506,10 @@
       <c r="D129" s="157" t="s">
         <v>1895</v>
       </c>
-      <c r="E129" s="201"/>
+      <c r="E129" s="213"/>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="191"/>
+      <c r="A130" s="194"/>
       <c r="B130" s="157" t="s">
         <v>2046</v>
       </c>
@@ -20508,7 +20522,7 @@
       <c r="E130" s="156"/>
     </row>
     <row r="131" spans="1:5">
-      <c r="A131" s="191"/>
+      <c r="A131" s="194"/>
       <c r="B131" s="157" t="s">
         <v>1896</v>
       </c>
@@ -20578,7 +20592,7 @@
     </row>
     <row r="136" spans="1:5" ht="99">
       <c r="A136" s="169"/>
-      <c r="B136" s="208" t="s">
+      <c r="B136" s="201" t="s">
         <v>2046</v>
       </c>
       <c r="C136" s="157" t="s">
@@ -20591,7 +20605,7 @@
     </row>
     <row r="137" spans="1:5" ht="33">
       <c r="A137" s="169"/>
-      <c r="B137" s="209"/>
+      <c r="B137" s="202"/>
       <c r="C137" s="157" t="s">
         <v>2051</v>
       </c>
@@ -20602,7 +20616,7 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="169"/>
-      <c r="B138" s="209"/>
+      <c r="B138" s="202"/>
       <c r="C138" s="157" t="s">
         <v>2052</v>
       </c>
@@ -20613,7 +20627,7 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="169"/>
-      <c r="B139" s="209"/>
+      <c r="B139" s="202"/>
       <c r="C139" s="157" t="s">
         <v>2053</v>
       </c>
@@ -20624,7 +20638,7 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="169"/>
-      <c r="B140" s="209"/>
+      <c r="B140" s="202"/>
       <c r="C140" s="157" t="s">
         <v>2054</v>
       </c>
@@ -20635,7 +20649,7 @@
     </row>
     <row r="141" spans="1:5" ht="33">
       <c r="A141" s="169"/>
-      <c r="B141" s="209"/>
+      <c r="B141" s="202"/>
       <c r="C141" s="157" t="s">
         <v>2055</v>
       </c>
@@ -20646,7 +20660,7 @@
     </row>
     <row r="142" spans="1:5" ht="33">
       <c r="A142" s="169"/>
-      <c r="B142" s="209"/>
+      <c r="B142" s="202"/>
       <c r="C142" s="157" t="s">
         <v>2056</v>
       </c>
@@ -20656,7 +20670,7 @@
       <c r="E142" s="163"/>
     </row>
     <row r="143" spans="1:5" ht="82.5">
-      <c r="B143" s="210"/>
+      <c r="B143" s="203"/>
       <c r="C143" s="151" t="s">
         <v>2079</v>
       </c>
@@ -20809,7 +20823,7 @@
       <c r="E153" s="163"/>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="191" t="s">
+      <c r="A154" s="194" t="s">
         <v>1825</v>
       </c>
       <c r="B154" s="157" t="s">
@@ -20821,10 +20835,10 @@
       <c r="D154" s="157" t="s">
         <v>1643</v>
       </c>
-      <c r="E154" s="197"/>
+      <c r="E154" s="209"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="191" t="str">
+      <c r="A155" s="194" t="str">
         <f>A154</f>
         <v>from_</v>
       </c>
@@ -20837,10 +20851,10 @@
       <c r="D155" s="157" t="s">
         <v>1902</v>
       </c>
-      <c r="E155" s="199"/>
+      <c r="E155" s="210"/>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="191" t="s">
+      <c r="A156" s="194" t="s">
         <v>1826</v>
       </c>
       <c r="B156" s="157" t="s">
@@ -20852,10 +20866,10 @@
       <c r="D156" s="157" t="s">
         <v>1643</v>
       </c>
-      <c r="E156" s="197"/>
+      <c r="E156" s="209"/>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="191" t="str">
+      <c r="A157" s="194" t="str">
         <f>A156</f>
         <v>to</v>
       </c>
@@ -20868,10 +20882,10 @@
       <c r="D157" s="157" t="s">
         <v>1902</v>
       </c>
-      <c r="E157" s="199"/>
+      <c r="E157" s="210"/>
     </row>
     <row r="158" spans="1:5">
-      <c r="A158" s="205" t="s">
+      <c r="A158" s="198" t="s">
         <v>1827</v>
       </c>
       <c r="B158" s="157" t="s">
@@ -20884,7 +20898,7 @@
       <c r="E158" s="163"/>
     </row>
     <row r="159" spans="1:5">
-      <c r="A159" s="207"/>
+      <c r="A159" s="200"/>
       <c r="B159" s="157"/>
       <c r="C159" s="157" t="s">
         <v>1879</v>
@@ -20895,7 +20909,7 @@
       <c r="E159" s="164"/>
     </row>
     <row r="160" spans="1:5">
-      <c r="A160" s="206"/>
+      <c r="A160" s="199"/>
       <c r="B160" s="157"/>
       <c r="C160" s="157" t="s">
         <v>2022</v>
@@ -21112,7 +21126,7 @@
       <c r="A175" s="153" t="s">
         <v>1985</v>
       </c>
-      <c r="B175" s="202" t="s">
+      <c r="B175" s="192" t="s">
         <v>1985</v>
       </c>
       <c r="C175" s="151" t="s">
@@ -21123,7 +21137,7 @@
       <c r="A176" s="153" t="s">
         <v>1987</v>
       </c>
-      <c r="B176" s="203"/>
+      <c r="B176" s="193"/>
       <c r="C176" s="151" t="s">
         <v>1996</v>
       </c>
@@ -21132,7 +21146,7 @@
       <c r="A177" s="153" t="s">
         <v>1988</v>
       </c>
-      <c r="B177" s="203"/>
+      <c r="B177" s="193"/>
       <c r="C177" s="151" t="s">
         <v>1997</v>
       </c>
@@ -21141,7 +21155,7 @@
       <c r="A178" s="153" t="s">
         <v>1989</v>
       </c>
-      <c r="B178" s="203"/>
+      <c r="B178" s="193"/>
       <c r="C178" s="151" t="s">
         <v>1998</v>
       </c>
@@ -21150,7 +21164,7 @@
       <c r="A179" s="153" t="s">
         <v>1990</v>
       </c>
-      <c r="B179" s="203"/>
+      <c r="B179" s="193"/>
       <c r="C179" s="151" t="s">
         <v>1999</v>
       </c>
@@ -21159,7 +21173,7 @@
       <c r="A180" s="153" t="s">
         <v>1991</v>
       </c>
-      <c r="B180" s="203"/>
+      <c r="B180" s="193"/>
       <c r="C180" s="151" t="s">
         <v>2000</v>
       </c>
@@ -21168,7 +21182,7 @@
       <c r="A181" s="153" t="s">
         <v>1992</v>
       </c>
-      <c r="B181" s="203"/>
+      <c r="B181" s="193"/>
       <c r="C181" s="151" t="s">
         <v>2001</v>
       </c>
@@ -21177,7 +21191,7 @@
       <c r="A182" s="153" t="s">
         <v>1993</v>
       </c>
-      <c r="B182" s="203"/>
+      <c r="B182" s="193"/>
       <c r="C182" s="151" t="s">
         <v>2002</v>
       </c>
@@ -21186,7 +21200,7 @@
       <c r="A183" s="153" t="s">
         <v>1994</v>
       </c>
-      <c r="B183" s="203"/>
+      <c r="B183" s="193"/>
       <c r="C183" s="151" t="s">
         <v>2003</v>
       </c>
@@ -21195,7 +21209,7 @@
       <c r="A184" s="153" t="s">
         <v>1995</v>
       </c>
-      <c r="B184" s="203"/>
+      <c r="B184" s="193"/>
       <c r="C184" s="151" t="s">
         <v>2004</v>
       </c>
@@ -21204,7 +21218,7 @@
       <c r="A185" s="153" t="s">
         <v>2230</v>
       </c>
-      <c r="B185" s="203"/>
+      <c r="B185" s="193"/>
       <c r="C185" s="151" t="s">
         <v>2225</v>
       </c>
@@ -21216,7 +21230,7 @@
       <c r="A186" s="153" t="s">
         <v>2231</v>
       </c>
-      <c r="B186" s="203"/>
+      <c r="B186" s="193"/>
       <c r="C186" s="151" t="s">
         <v>2226</v>
       </c>
@@ -21228,7 +21242,7 @@
       <c r="A187" s="153" t="s">
         <v>2232</v>
       </c>
-      <c r="B187" s="203"/>
+      <c r="B187" s="193"/>
       <c r="C187" s="151" t="s">
         <v>2227</v>
       </c>
@@ -21240,7 +21254,7 @@
       <c r="A188" s="153" t="s">
         <v>2233</v>
       </c>
-      <c r="B188" s="203"/>
+      <c r="B188" s="193"/>
       <c r="C188" s="151" t="s">
         <v>2228</v>
       </c>
@@ -21252,7 +21266,7 @@
       <c r="A189" s="153" t="s">
         <v>2234</v>
       </c>
-      <c r="B189" s="203"/>
+      <c r="B189" s="193"/>
       <c r="C189" s="151" t="s">
         <v>2229</v>
       </c>
@@ -21264,7 +21278,7 @@
       <c r="A190" s="153" t="s">
         <v>2235</v>
       </c>
-      <c r="B190" s="203"/>
+      <c r="B190" s="193"/>
       <c r="C190" s="151" t="s">
         <v>2238</v>
       </c>
@@ -21276,7 +21290,7 @@
       <c r="A191" s="153" t="s">
         <v>2236</v>
       </c>
-      <c r="B191" s="203"/>
+      <c r="B191" s="193"/>
       <c r="C191" s="151" t="s">
         <v>2239</v>
       </c>
@@ -21288,7 +21302,7 @@
       <c r="A192" s="153" t="s">
         <v>2237</v>
       </c>
-      <c r="B192" s="203"/>
+      <c r="B192" s="193"/>
       <c r="C192" s="151" t="s">
         <v>2240</v>
       </c>
@@ -21300,7 +21314,7 @@
       <c r="A193" s="153" t="s">
         <v>2244</v>
       </c>
-      <c r="B193" s="203"/>
+      <c r="B193" s="193"/>
       <c r="C193" s="151" t="s">
         <v>2247</v>
       </c>
@@ -21309,7 +21323,7 @@
       <c r="A194" s="153" t="s">
         <v>2245</v>
       </c>
-      <c r="B194" s="203"/>
+      <c r="B194" s="193"/>
       <c r="C194" s="151" t="s">
         <v>2248</v>
       </c>
@@ -21318,7 +21332,7 @@
       <c r="A195" s="153" t="s">
         <v>2246</v>
       </c>
-      <c r="B195" s="203"/>
+      <c r="B195" s="193"/>
       <c r="C195" s="151" t="s">
         <v>2249</v>
       </c>
@@ -21327,7 +21341,7 @@
       <c r="A196" s="153" t="s">
         <v>2250</v>
       </c>
-      <c r="B196" s="203"/>
+      <c r="B196" s="193"/>
       <c r="C196" s="151" t="s">
         <v>2251</v>
       </c>
@@ -21336,7 +21350,7 @@
       <c r="A197" s="153" t="s">
         <v>2252</v>
       </c>
-      <c r="B197" s="203"/>
+      <c r="B197" s="193"/>
       <c r="C197" s="151" t="s">
         <v>2257</v>
       </c>
@@ -21345,7 +21359,7 @@
       <c r="A198" s="153" t="s">
         <v>2253</v>
       </c>
-      <c r="B198" s="203"/>
+      <c r="B198" s="193"/>
       <c r="C198" s="151" t="s">
         <v>2258</v>
       </c>
@@ -21354,7 +21368,7 @@
       <c r="A199" s="153" t="s">
         <v>2254</v>
       </c>
-      <c r="B199" s="203"/>
+      <c r="B199" s="193"/>
       <c r="C199" s="151" t="s">
         <v>2259</v>
       </c>
@@ -21363,7 +21377,7 @@
       <c r="A200" s="153" t="s">
         <v>2255</v>
       </c>
-      <c r="B200" s="203"/>
+      <c r="B200" s="193"/>
       <c r="C200" s="151" t="s">
         <v>2260</v>
       </c>
@@ -21372,7 +21386,7 @@
       <c r="A201" s="153" t="s">
         <v>2256</v>
       </c>
-      <c r="B201" s="203"/>
+      <c r="B201" s="193"/>
       <c r="C201" s="151" t="s">
         <v>2262</v>
       </c>
@@ -21381,7 +21395,7 @@
       <c r="A202" s="153" t="s">
         <v>2266</v>
       </c>
-      <c r="B202" s="203"/>
+      <c r="B202" s="193"/>
       <c r="C202" s="151" t="s">
         <v>2267</v>
       </c>
@@ -21390,7 +21404,7 @@
       <c r="A203" s="153" t="s">
         <v>2270</v>
       </c>
-      <c r="B203" s="203"/>
+      <c r="B203" s="193"/>
       <c r="C203" s="151" t="s">
         <v>2271</v>
       </c>
@@ -21399,13 +21413,13 @@
       <c r="A204" s="153" t="s">
         <v>2263</v>
       </c>
-      <c r="B204" s="203"/>
+      <c r="B204" s="193"/>
       <c r="C204" s="151" t="s">
         <v>2264</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="198">
-      <c r="B205" s="203"/>
+      <c r="B205" s="193"/>
       <c r="C205" s="151" t="s">
         <v>2261</v>
       </c>
@@ -21414,7 +21428,7 @@
       <c r="A206" s="153" t="s">
         <v>2265</v>
       </c>
-      <c r="B206" s="203"/>
+      <c r="B206" s="193"/>
       <c r="C206" s="151" t="s">
         <v>2268</v>
       </c>
@@ -21423,13 +21437,13 @@
       </c>
     </row>
     <row r="207" spans="1:4">
-      <c r="B207" s="203"/>
+      <c r="B207" s="193"/>
       <c r="C207" s="151" t="s">
         <v>2272</v>
       </c>
     </row>
     <row r="208" spans="1:4">
-      <c r="B208" s="204"/>
+      <c r="B208" s="197"/>
     </row>
     <row r="209" spans="1:4" ht="33">
       <c r="A209" s="153" t="s">
@@ -21530,7 +21544,7 @@
       <c r="A216" s="153" t="s">
         <v>2064</v>
       </c>
-      <c r="B216" s="202" t="s">
+      <c r="B216" s="192" t="s">
         <v>2046</v>
       </c>
       <c r="C216" s="151" t="s">
@@ -21541,7 +21555,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" ht="33">
-      <c r="B217" s="203"/>
+      <c r="B217" s="193"/>
       <c r="C217" s="151" t="s">
         <v>2066</v>
       </c>
@@ -22047,20 +22061,17 @@
   </sheetData>
   <autoFilter ref="A1:D166"/>
   <mergeCells count="43">
-    <mergeCell ref="B216:B217"/>
-    <mergeCell ref="A44:A54"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A61:A74"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="A103:A109"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="B175:B208"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="A6:A30"/>
+    <mergeCell ref="E6:E30"/>
+    <mergeCell ref="E34:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E91:E96"/>
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="E103:E109"/>
+    <mergeCell ref="E111:E114"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="E128:E129"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A158:A160"/>
     <mergeCell ref="B136:B143"/>
@@ -22077,19 +22088,22 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="E156:E157"/>
     <mergeCell ref="A128:A131"/>
+    <mergeCell ref="B216:B217"/>
+    <mergeCell ref="A44:A54"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A61:A74"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="A103:A109"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="B175:B208"/>
     <mergeCell ref="B118:B121"/>
     <mergeCell ref="A118:A121"/>
-    <mergeCell ref="E88:E90"/>
-    <mergeCell ref="E103:E109"/>
-    <mergeCell ref="E111:E114"/>
-    <mergeCell ref="E118:E121"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="A6:A30"/>
-    <mergeCell ref="E6:E30"/>
-    <mergeCell ref="E34:E38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="E91:E96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -22100,8 +22114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E593"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D251" sqref="D251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -22147,10 +22161,10 @@
     </row>
     <row r="5" spans="1:4" ht="68.25" customHeight="1">
       <c r="A5" s="50"/>
-      <c r="B5" s="220" t="s">
+      <c r="B5" s="218" t="s">
         <v>1381</v>
       </c>
-      <c r="C5" s="220"/>
+      <c r="C5" s="218"/>
       <c r="D5" s="94"/>
     </row>
     <row r="6" spans="1:4" ht="66">
@@ -22262,20 +22276,20 @@
       <c r="A16" s="132" t="s">
         <v>1442</v>
       </c>
-      <c r="B16" s="221" t="s">
+      <c r="B16" s="219" t="s">
         <v>1443</v>
       </c>
-      <c r="C16" s="221"/>
+      <c r="C16" s="219"/>
       <c r="D16" s="96"/>
     </row>
     <row r="17" spans="1:4" ht="87.75" customHeight="1">
       <c r="A17" s="132" t="s">
         <v>1444</v>
       </c>
-      <c r="B17" s="221" t="s">
+      <c r="B17" s="219" t="s">
         <v>1445</v>
       </c>
-      <c r="C17" s="221"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="96"/>
     </row>
     <row r="18" spans="1:4">
@@ -22357,7 +22371,7 @@
       <c r="D27" s="96"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="217" t="s">
+      <c r="A28" s="220" t="s">
         <v>1211</v>
       </c>
       <c r="B28" s="106" t="s">
@@ -22366,33 +22380,33 @@
       <c r="D28" s="96"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="217"/>
+      <c r="A29" s="220"/>
       <c r="B29" s="106"/>
       <c r="D29" s="96"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="217"/>
+      <c r="A30" s="220"/>
       <c r="B30" s="13" t="s">
         <v>1213</v>
       </c>
       <c r="D30" s="96"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="217"/>
+      <c r="A31" s="220"/>
       <c r="B31" s="77" t="s">
         <v>1214</v>
       </c>
       <c r="D31" s="96"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="217"/>
+      <c r="A32" s="220"/>
       <c r="B32" s="13" t="s">
         <v>1215</v>
       </c>
       <c r="D32" s="96"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="217"/>
+      <c r="A33" s="220"/>
       <c r="B33" s="106"/>
       <c r="D33" s="96"/>
     </row>
@@ -22415,7 +22429,7 @@
       <c r="D35" s="96"/>
     </row>
     <row r="36" spans="1:4" ht="49.5">
-      <c r="A36" s="217" t="s">
+      <c r="A36" s="220" t="s">
         <v>1220</v>
       </c>
       <c r="B36" s="106" t="s">
@@ -22424,33 +22438,33 @@
       <c r="D36" s="96"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="217"/>
+      <c r="A37" s="220"/>
       <c r="B37" s="106"/>
       <c r="D37" s="96"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="217"/>
+      <c r="A38" s="220"/>
       <c r="B38" s="13" t="s">
         <v>1222</v>
       </c>
       <c r="D38" s="96"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="217"/>
+      <c r="A39" s="220"/>
       <c r="B39" s="13" t="s">
         <v>1223</v>
       </c>
       <c r="D39" s="96"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="217"/>
+      <c r="A40" s="220"/>
       <c r="B40" s="13" t="s">
         <v>1224</v>
       </c>
       <c r="D40" s="96"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="217"/>
+      <c r="A41" s="220"/>
       <c r="B41" s="106"/>
       <c r="D41" s="96"/>
     </row>
@@ -22480,7 +22494,7 @@
       <c r="D44" s="96"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="217" t="s">
+      <c r="A45" s="220" t="s">
         <v>1230</v>
       </c>
       <c r="B45" s="106" t="s">
@@ -22489,31 +22503,31 @@
       <c r="D45" s="96"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="217"/>
+      <c r="A46" s="220"/>
       <c r="B46" s="106"/>
       <c r="D46" s="96"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="217"/>
+      <c r="A47" s="220"/>
       <c r="B47" s="13" t="s">
         <v>1232</v>
       </c>
       <c r="D47" s="96"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="217"/>
+      <c r="A48" s="220"/>
       <c r="B48" s="77" t="s">
         <v>1233</v>
       </c>
       <c r="D48" s="96"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="217"/>
+      <c r="A49" s="220"/>
       <c r="B49" s="106"/>
       <c r="D49" s="96"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="217" t="s">
+      <c r="A50" s="220" t="s">
         <v>1234</v>
       </c>
       <c r="B50" s="106" t="s">
@@ -22522,45 +22536,45 @@
       <c r="D50" s="96"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="217"/>
+      <c r="A51" s="220"/>
       <c r="B51" s="106"/>
       <c r="D51" s="96"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="217"/>
+      <c r="A52" s="220"/>
       <c r="B52" s="13" t="s">
         <v>1236</v>
       </c>
       <c r="D52" s="96"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="217"/>
+      <c r="A53" s="220"/>
       <c r="B53" s="78" t="s">
         <v>1237</v>
       </c>
       <c r="D53" s="96"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="217"/>
+      <c r="A54" s="220"/>
       <c r="B54" s="79" t="s">
         <v>1238</v>
       </c>
       <c r="D54" s="96"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="217"/>
+      <c r="A55" s="220"/>
       <c r="B55" s="78" t="s">
         <v>1239</v>
       </c>
       <c r="D55" s="96"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="217"/>
+      <c r="A56" s="220"/>
       <c r="B56" s="106"/>
       <c r="D56" s="96"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="217" t="s">
+      <c r="A57" s="220" t="s">
         <v>1240</v>
       </c>
       <c r="B57" s="106" t="s">
@@ -22569,24 +22583,24 @@
       <c r="D57" s="96"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="217"/>
+      <c r="A58" s="220"/>
       <c r="B58" s="106"/>
       <c r="D58" s="96"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="217"/>
+      <c r="A59" s="220"/>
       <c r="B59" s="13" t="s">
         <v>1242</v>
       </c>
       <c r="D59" s="96"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="217"/>
+      <c r="A60" s="220"/>
       <c r="B60" s="106"/>
       <c r="D60" s="96"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="217"/>
+      <c r="A61" s="220"/>
       <c r="B61" s="106"/>
       <c r="D61" s="96"/>
     </row>
@@ -22672,7 +22686,7 @@
       <c r="D71" s="96"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="217" t="s">
+      <c r="A72" s="220" t="s">
         <v>1391</v>
       </c>
       <c r="B72" s="106" t="s">
@@ -22681,24 +22695,24 @@
       <c r="D72" s="96"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="217"/>
+      <c r="A73" s="220"/>
       <c r="B73" s="106"/>
       <c r="D73" s="96"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="217"/>
+      <c r="A74" s="220"/>
       <c r="B74" s="13" t="s">
         <v>1257</v>
       </c>
       <c r="D74" s="96"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="217"/>
+      <c r="A75" s="220"/>
       <c r="B75" s="106"/>
       <c r="D75" s="96"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="217" t="s">
+      <c r="A76" s="220" t="s">
         <v>1393</v>
       </c>
       <c r="B76" s="106" t="s">
@@ -22707,31 +22721,31 @@
       <c r="D76" s="96"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="217"/>
+      <c r="A77" s="220"/>
       <c r="B77" s="106"/>
       <c r="D77" s="96"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="217"/>
+      <c r="A78" s="220"/>
       <c r="B78" s="77" t="s">
         <v>1258</v>
       </c>
       <c r="D78" s="96"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="217"/>
+      <c r="A79" s="220"/>
       <c r="B79" s="80" t="s">
         <v>1259</v>
       </c>
       <c r="D79" s="96"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="217"/>
+      <c r="A80" s="220"/>
       <c r="B80" s="106"/>
       <c r="D80" s="96"/>
     </row>
     <row r="81" spans="1:4" ht="33">
-      <c r="A81" s="217" t="s">
+      <c r="A81" s="220" t="s">
         <v>1395</v>
       </c>
       <c r="B81" s="106" t="s">
@@ -22740,68 +22754,68 @@
       <c r="D81" s="96"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="217"/>
+      <c r="A82" s="220"/>
       <c r="B82" s="106"/>
       <c r="D82" s="96"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="217"/>
+      <c r="A83" s="220"/>
       <c r="B83" s="106" t="s">
         <v>1574</v>
       </c>
       <c r="D83" s="96"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="217"/>
+      <c r="A84" s="220"/>
       <c r="B84" s="81" t="s">
         <v>1260</v>
       </c>
       <c r="D84" s="96"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="217"/>
+      <c r="A85" s="220"/>
       <c r="B85" s="77" t="s">
         <v>1261</v>
       </c>
       <c r="D85" s="96"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="217"/>
+      <c r="A86" s="220"/>
       <c r="B86" s="77" t="s">
         <v>1262</v>
       </c>
       <c r="D86" s="96"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="217"/>
+      <c r="A87" s="220"/>
       <c r="B87" s="77" t="s">
         <v>1263</v>
       </c>
       <c r="D87" s="96"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="217"/>
+      <c r="A88" s="220"/>
       <c r="B88" s="77" t="s">
         <v>1264</v>
       </c>
       <c r="D88" s="96"/>
     </row>
     <row r="89" spans="1:4" ht="33">
-      <c r="A89" s="217"/>
+      <c r="A89" s="220"/>
       <c r="B89" s="106" t="s">
         <v>1572</v>
       </c>
       <c r="D89" s="96"/>
     </row>
     <row r="90" spans="1:4" ht="49.5">
-      <c r="A90" s="217"/>
+      <c r="A90" s="220"/>
       <c r="B90" s="106" t="s">
         <v>1573</v>
       </c>
       <c r="D90" s="96"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="217" t="s">
+      <c r="A91" s="220" t="s">
         <v>1397</v>
       </c>
       <c r="B91" s="106" t="s">
@@ -22810,40 +22824,40 @@
       <c r="D91" s="96"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="217"/>
+      <c r="A92" s="220"/>
       <c r="B92" s="106"/>
       <c r="D92" s="96"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="217"/>
+      <c r="A93" s="220"/>
       <c r="B93" s="13" t="s">
         <v>1265</v>
       </c>
       <c r="D93" s="96"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="217"/>
+      <c r="A94" s="220"/>
       <c r="B94" s="13" t="s">
         <v>1266</v>
       </c>
       <c r="D94" s="96"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="217"/>
+      <c r="A95" s="220"/>
       <c r="B95" s="77" t="s">
         <v>1267</v>
       </c>
       <c r="D95" s="96"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="217"/>
+      <c r="A96" s="220"/>
       <c r="B96" s="106" t="s">
         <v>1571</v>
       </c>
       <c r="D96" s="96"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="217" t="s">
+      <c r="A97" s="220" t="s">
         <v>1399</v>
       </c>
       <c r="B97" s="106" t="s">
@@ -22852,31 +22866,31 @@
       <c r="D97" s="96"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="217"/>
+      <c r="A98" s="220"/>
       <c r="B98" s="106"/>
       <c r="D98" s="96"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="217"/>
+      <c r="A99" s="220"/>
       <c r="B99" s="77" t="s">
         <v>1268</v>
       </c>
       <c r="D99" s="96"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="217"/>
+      <c r="A100" s="220"/>
       <c r="B100" s="80" t="s">
         <v>1269</v>
       </c>
       <c r="D100" s="96"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="217"/>
+      <c r="A101" s="220"/>
       <c r="B101" s="106"/>
       <c r="D101" s="96"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="217" t="s">
+      <c r="A102" s="220" t="s">
         <v>1401</v>
       </c>
       <c r="B102" s="106" t="s">
@@ -22885,26 +22899,26 @@
       <c r="D102" s="96"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="217"/>
+      <c r="A103" s="220"/>
       <c r="B103" s="106"/>
       <c r="D103" s="96"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="217"/>
+      <c r="A104" s="220"/>
       <c r="B104" s="77" t="s">
         <v>1270</v>
       </c>
       <c r="D104" s="96"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="217"/>
+      <c r="A105" s="220"/>
       <c r="B105" s="80" t="s">
         <v>1271</v>
       </c>
       <c r="D105" s="96"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="217"/>
+      <c r="A106" s="220"/>
       <c r="B106" s="106"/>
       <c r="D106" s="96"/>
     </row>
@@ -22916,7 +22930,7 @@
       <c r="D107" s="96"/>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="217" t="s">
+      <c r="A108" s="220" t="s">
         <v>1272</v>
       </c>
       <c r="B108" s="106" t="s">
@@ -22925,55 +22939,55 @@
       <c r="D108" s="96"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="217"/>
+      <c r="A109" s="220"/>
       <c r="B109" s="106"/>
       <c r="D109" s="96"/>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="217"/>
+      <c r="A110" s="220"/>
       <c r="B110" s="106"/>
       <c r="D110" s="96"/>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="217"/>
+      <c r="A111" s="220"/>
       <c r="B111" s="13" t="s">
         <v>1273</v>
       </c>
       <c r="D111" s="96"/>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="217"/>
+      <c r="A112" s="220"/>
       <c r="B112" s="82" t="s">
         <v>1274</v>
       </c>
       <c r="D112" s="96"/>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="217"/>
+      <c r="A113" s="220"/>
       <c r="B113" s="13" t="s">
         <v>1275</v>
       </c>
       <c r="D113" s="96"/>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="217"/>
+      <c r="A114" s="220"/>
       <c r="B114" s="82" t="s">
         <v>1276</v>
       </c>
       <c r="D114" s="96"/>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="217"/>
+      <c r="A115" s="220"/>
       <c r="B115" s="106"/>
       <c r="D115" s="96"/>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="217"/>
+      <c r="A116" s="220"/>
       <c r="B116" s="106"/>
       <c r="D116" s="96"/>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="219" t="s">
+      <c r="A117" s="222" t="s">
         <v>1277</v>
       </c>
       <c r="B117" s="106" t="s">
@@ -22982,33 +22996,33 @@
       <c r="D117" s="96"/>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="219"/>
+      <c r="A118" s="222"/>
       <c r="B118" s="106"/>
       <c r="D118" s="96"/>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="219"/>
+      <c r="A119" s="222"/>
       <c r="B119" s="13" t="s">
         <v>1278</v>
       </c>
       <c r="D119" s="96"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="219"/>
+      <c r="A120" s="222"/>
       <c r="B120" s="77" t="s">
         <v>1279</v>
       </c>
       <c r="D120" s="96"/>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="219"/>
+      <c r="A121" s="222"/>
       <c r="B121" s="82" t="s">
         <v>1280</v>
       </c>
       <c r="D121" s="96"/>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="219"/>
+      <c r="A122" s="222"/>
       <c r="B122" s="106"/>
       <c r="D122" s="96"/>
     </row>
@@ -24324,7 +24338,7 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" s="115"/>
-      <c r="B279" s="218" t="s">
+      <c r="B279" s="221" t="s">
         <v>720</v>
       </c>
       <c r="C279" s="106" t="s">
@@ -24334,7 +24348,7 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="115"/>
-      <c r="B280" s="218"/>
+      <c r="B280" s="221"/>
       <c r="C280" s="106" t="s">
         <v>722</v>
       </c>
@@ -24342,7 +24356,7 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="115"/>
-      <c r="B281" s="218"/>
+      <c r="B281" s="221"/>
       <c r="C281" s="106" t="s">
         <v>723</v>
       </c>
@@ -24350,7 +24364,7 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="115"/>
-      <c r="B282" s="218"/>
+      <c r="B282" s="221"/>
       <c r="C282" s="106" t="s">
         <v>724</v>
       </c>
@@ -24358,7 +24372,7 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" s="115"/>
-      <c r="B283" s="218"/>
+      <c r="B283" s="221"/>
       <c r="C283" s="116" t="s">
         <v>725</v>
       </c>
@@ -24366,7 +24380,7 @@
     </row>
     <row r="284" spans="1:4" ht="66">
       <c r="A284" s="115"/>
-      <c r="B284" s="218"/>
+      <c r="B284" s="221"/>
       <c r="C284" s="106" t="s">
         <v>1623</v>
       </c>
@@ -24376,7 +24390,7 @@
     </row>
     <row r="285" spans="1:4" ht="49.5">
       <c r="A285" s="115"/>
-      <c r="B285" s="218"/>
+      <c r="B285" s="221"/>
       <c r="C285" s="106" t="s">
         <v>1620</v>
       </c>
@@ -24386,7 +24400,7 @@
     </row>
     <row r="286" spans="1:4" ht="33">
       <c r="A286" s="115"/>
-      <c r="B286" s="218"/>
+      <c r="B286" s="221"/>
       <c r="C286" s="106" t="s">
         <v>726</v>
       </c>
@@ -26829,6 +26843,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A81:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="B279:B286"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A108:A116"/>
+    <mergeCell ref="A117:A122"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
@@ -26839,13 +26860,6 @@
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A81:A90"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="B279:B286"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="A108:A116"/>
-    <mergeCell ref="A117:A122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -28803,13 +28817,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1">
-      <c r="A18" s="222" t="s">
+      <c r="A18" s="223" t="s">
         <v>1030</v>
       </c>
-      <c r="B18" s="222"/>
-      <c r="C18" s="222"/>
-      <c r="D18" s="222"/>
-      <c r="E18" s="222"/>
+      <c r="B18" s="223"/>
+      <c r="C18" s="223"/>
+      <c r="D18" s="223"/>
+      <c r="E18" s="223"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28908,8 +28922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29242,9 +29256,12 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" ht="75">
       <c r="A55" s="64" t="s">
         <v>1010</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>2294</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -29252,9 +29269,12 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" ht="75">
       <c r="A57" s="64" t="s">
         <v>1016</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>2295</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -29438,7 +29458,9 @@
       <c r="A86" s="140" t="s">
         <v>979</v>
       </c>
-      <c r="B86" s="106"/>
+      <c r="B86" s="186" t="s">
+        <v>2296</v>
+      </c>
       <c r="C86" s="106"/>
     </row>
     <row r="87" spans="1:3" ht="16.5">

</xml_diff>